<commit_message>
Mise à jour à la fin de tous les premiers matchs de poules
</commit_message>
<xml_diff>
--- a/Results_20180606.xlsx
+++ b/Results_20180606.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dompd\Document\worldcup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160B011D-865A-4E59-B132-BCF7C790B2B7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC63D4B-3BC9-492B-BC3B-DD5DA0E6F08B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="6570" tabRatio="747" activeTab="9" xr2:uid="{E93A372B-1490-4A28-B29E-3CD0AFC460B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="6570" tabRatio="747" activeTab="10" xr2:uid="{E93A372B-1490-4A28-B29E-3CD0AFC460B9}"/>
   </bookViews>
   <sheets>
     <sheet name="GivenZeroEloNewProbaNumpyF" sheetId="13" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="20180619" sheetId="19" r:id="rId8"/>
     <sheet name="20180621" sheetId="20" r:id="rId9"/>
     <sheet name="20180623" sheetId="21" r:id="rId10"/>
+    <sheet name="20180624" sheetId="22" r:id="rId11"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5507" uniqueCount="1392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5734" uniqueCount="1431">
   <si>
     <t xml:space="preserve"> 1M  </t>
   </si>
@@ -4210,6 +4211,123 @@
   </si>
   <si>
     <t xml:space="preserve"> 2401   24   4.2  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  0     0    0,0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5896   59   1,7  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4104   41   2,4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 482    5    20,7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2873   29   3,5  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6645   66   1,5  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1657   17   6,0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4988   50   2,0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3355   34   3,0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2626   26   3,8  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7374   74   1,4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1460   15   6,8  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5914   59   1,7  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9916   99   1,0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  84    1   119,0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5171   52   1,9  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 643    6    15,6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4102   41   2,4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7266   73   1,4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 364    4    27,5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2370   24   4,2  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1865   19   5,4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 923    9    10,8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7212   72   1,4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1098   11   9,1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8021   80   1,2  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 881    9    11,4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6569   66   1,5  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 650    6    15,4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1310   13   7,6  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1471   15   6,8  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6242   62   1,6  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3758   38   2,7  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3362   34   3,0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3723   37   2,7  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2915   29   3,4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3259   33   3,1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3401   34   2,9  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3340   33   3,0  </t>
   </si>
 </sst>
 </file>
@@ -4294,7 +4412,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -4371,7 +4492,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9347FB5C-412B-40E4-B41C-02A6FE0AE109}" name="Tableau8" displayName="Tableau8" ref="A35:P83" totalsRowShown="0">
   <autoFilter ref="A35:P83" xr:uid="{EDDAA4B0-4193-4019-AE5F-84EBF522F9B7}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{43B17E18-2CA7-4710-A569-99665BF192B8}" name="Date       " dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{43B17E18-2CA7-4710-A569-99665BF192B8}" name="Date       " dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{18B91E56-AB03-41DF-8AA6-39846E8A232D}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{61520696-7ABA-491A-B0E9-DC64F7B4D675}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{DAF25AD3-8A89-40EA-9E2E-304087E594D0}" name=" Team2             "/>
@@ -4443,7 +4564,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7C38957E-D3C3-4EDE-8C2B-17F0C9D00713}" name="Tableau13" displayName="Tableau13" ref="A35:P83" totalsRowShown="0">
   <autoFilter ref="A35:P83" xr:uid="{0D6341F4-3D48-495C-9EA8-AE26D5F92808}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{51876778-EE60-4DB5-807C-3BAF31F3EBA7}" name="Date       " dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{51876778-EE60-4DB5-807C-3BAF31F3EBA7}" name="Date       " dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{355B6899-F63D-4BB3-AC20-86507223A1DE}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{5B238E8D-5A42-4AA8-8DDA-0E8C007BEA13}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{7415F0D1-2339-4094-B4CA-DA1E67C3B8EA}" name=" Team2             "/>
@@ -4513,7 +4634,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CE74AF0B-2793-4D5F-AB14-98A0B7A5496B}" name="Tableau16" displayName="Tableau16" ref="A35:O67" totalsRowShown="0">
   <autoFilter ref="A35:O67" xr:uid="{69E73736-E9F1-4F73-A95D-947FCB875A43}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{0392F536-43A6-4135-BEBC-512373D21627}" name="Date       " dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{0392F536-43A6-4135-BEBC-512373D21627}" name="Date       " dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{7BAB4429-37F6-4193-A8F8-F41D34E505D6}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{3B193FBE-751B-4A4F-93E2-DF4A408FB3D8}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{6284F227-005C-4A09-AA27-A79FD219F58E}" name=" Team2             "/>
@@ -4568,7 +4689,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{F69BDF94-37F3-4256-A51D-135B8671BBA5}" name="Tableau18" displayName="Tableau18" ref="A35:O60" totalsRowShown="0">
   <autoFilter ref="A35:O60" xr:uid="{C72E9688-1DB9-4326-AAFD-05173885C691}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{3CBB2762-D6F0-4569-9979-8C76659F6CC5}" name="Date       " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{3CBB2762-D6F0-4569-9979-8C76659F6CC5}" name="Date       " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{BFA086CA-AE8D-4E23-AC75-DD0FDDD097DA}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{3F61DBAB-FA0F-4F11-A4D7-7FA6D75A7595}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{E27010C3-F9B7-4499-A5E2-1EC7EB737B35}" name=" Team2             "/>
@@ -4623,7 +4744,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D407DA2-1E3C-4BF9-9DEE-6FB85EA50B45}" name="Tableau11" displayName="Tableau11" ref="A1:M49" totalsRowShown="0">
   <autoFilter ref="A1:M49" xr:uid="{23AFB364-C990-4A52-88E8-7FFEF3078878}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{715799BB-9DC7-47F7-B86F-82ABC24CB807}" name="Date       " dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{715799BB-9DC7-47F7-B86F-82ABC24CB807}" name="Date       " dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{4203B992-4E6D-4429-85EA-C12615438D81}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{BFDE9085-79AD-4E69-824A-7F37EFD0712D}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{C450FEF0-7D71-4ABC-98B4-BB1C92D77557}" name=" Team2             "/>
@@ -4645,7 +4766,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{A8D74ED4-D634-440E-B79D-A0CECB3D0BB4}" name="Tableau20" displayName="Tableau20" ref="A35:O57" totalsRowShown="0">
   <autoFilter ref="A35:O57" xr:uid="{DBC3BA96-1AEA-4E50-8EFB-3B8F2A65E034}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{505A2FAA-9C6E-4FAA-AFF9-AEB929DD9CC6}" name="Date       " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{505A2FAA-9C6E-4FAA-AFF9-AEB929DD9CC6}" name="Date       " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{867A407D-4178-4402-A799-18F5A03E371D}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{7861AA1D-8038-4664-9ADF-6B396876114D}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{55DE77B8-DAE3-4901-9AB5-4C62EB2FDE99}" name=" Team2             "/>
@@ -4662,6 +4783,62 @@
     <tableColumn id="15" xr3:uid="{DC60B1FB-2774-42C7-898D-E994B4D29FFB}" name="  2G   "/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7089D5EB-82AB-4559-BE4B-61E1D3CA6A63}" name="Tableau22" displayName="Tableau22" ref="A27:P43" totalsRowShown="0">
+  <autoFilter ref="A27:P43" xr:uid="{524D6DE2-B53E-4BBA-8981-8113AD62C0B8}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{9C67B6D3-D448-4651-BD7D-389542AC0269}" name="Date       " dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{3B559211-2D70-475D-8EA0-7AC81A7824E8}" name="    Code    "/>
+    <tableColumn id="3" xr3:uid="{37269AF9-F2D2-4764-A769-81F3DE821B5F}" name=" Team1             "/>
+    <tableColumn id="4" xr3:uid="{EF245AAD-278C-436F-B4BE-1841C2C25E47}" name=" Team2             "/>
+    <tableColumn id="5" xr3:uid="{A7A19ABF-CBDC-4DAC-9E65-994D8CD3C45B}" name="1"/>
+    <tableColumn id="6" xr3:uid="{93108BC1-E2A1-4F7F-A493-088F090D0F3E}" name="  N  "/>
+    <tableColumn id="7" xr3:uid="{87BAA2ED-5C91-4C05-9F3B-A80A3EF5DF26}" name="2"/>
+    <tableColumn id="8" xr3:uid="{C5718FA4-E382-468F-AD10-5D7E3FF8B8A4}" name="  p1   "/>
+    <tableColumn id="9" xr3:uid="{62A589DE-AB69-4F7A-A4CF-9EFB1BCB4BF8}" name="  pN   "/>
+    <tableColumn id="10" xr3:uid="{737EF27A-C932-4B5B-A212-D8235A6D243B}" name="  p2   "/>
+    <tableColumn id="11" xr3:uid="{9BCC045C-9C3E-4691-82C0-423A4FE211F5}" name="  c1   "/>
+    <tableColumn id="12" xr3:uid="{293C673E-5359-47C3-9897-23093D63DAD9}" name="  cN   "/>
+    <tableColumn id="13" xr3:uid="{A27DE363-B524-42D3-9021-922FF358F320}" name="  C2   "/>
+    <tableColumn id="14" xr3:uid="{0E79C5E8-9FC7-45C9-953B-BF36B82064E5}" name="  1G   "/>
+    <tableColumn id="15" xr3:uid="{D8FDE262-64F1-4B7F-8148-07F4E82B6E16}" name="  2G   "/>
+    <tableColumn id="16" xr3:uid="{B150B2F2-7B5E-4A7B-A45A-608B75328EE5}" name="Colonne1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{24B410F9-CA56-4612-947E-B4C117F444F3}" name="Tableau21" displayName="Tableau21" ref="A1:S25" totalsRowShown="0">
+  <autoFilter ref="A1:S25" xr:uid="{7F3E1240-2FF9-4213-BF76-689F673C6E52}"/>
+  <sortState ref="A2:S25">
+    <sortCondition descending="1" ref="B1:B25"/>
+  </sortState>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{8D23A30F-2E6A-4BC7-89C2-388F11118DD8}" name="       Teams        "/>
+    <tableColumn id="2" xr3:uid="{CCE129C6-A2CF-490F-BF39-3B768E90E0F4}" name="1"/>
+    <tableColumn id="3" xr3:uid="{4390194A-93CC-44C6-919D-C6A0D36786F6}" name=" 1M  "/>
+    <tableColumn id="4" xr3:uid="{6235FBFA-1BB7-4A09-BEFC-4712D99320EB}" name="2"/>
+    <tableColumn id="5" xr3:uid="{C6839D61-199F-4BB9-8259-24C2BAC57277}" name="4"/>
+    <tableColumn id="6" xr3:uid="{D23DCC58-BE6E-4E6C-9629-51D47F1305B3}" name="8"/>
+    <tableColumn id="7" xr3:uid="{9B7BECED-ED2E-4294-8C9D-BE0BE8E4EB09}" name=" q8  "/>
+    <tableColumn id="8" xr3:uid="{5E346E0D-70DD-443B-AE7B-157296BD698E}" name="  p1   "/>
+    <tableColumn id="9" xr3:uid="{6EA21671-F212-496D-A7EE-BF094201D52A}" name="  p1M  "/>
+    <tableColumn id="10" xr3:uid="{ED2284C1-7053-4DE7-8DFF-7E130BDE886E}" name="  p2   "/>
+    <tableColumn id="11" xr3:uid="{D2B99565-F48A-4D15-B095-C60D05629A62}" name="  p4   "/>
+    <tableColumn id="12" xr3:uid="{C5B4A4E7-0743-4C3A-B6A6-B33CAB18C283}" name="  p8   "/>
+    <tableColumn id="13" xr3:uid="{288C3980-CA5F-4BFE-A23E-5DFE8446EB56}" name="  pq8  "/>
+    <tableColumn id="14" xr3:uid="{40049FDF-FB7B-486B-962A-4422F37CC17F}" name="  c1   "/>
+    <tableColumn id="15" xr3:uid="{ADE313DF-0D50-4491-B312-00201F562DFC}" name="  c1M  "/>
+    <tableColumn id="16" xr3:uid="{C5B7F4BC-317A-48F6-BA65-F2C83694FB89}" name="  c2   "/>
+    <tableColumn id="17" xr3:uid="{D8C14BBB-A0D0-4CE6-8EC3-EB41974B008C}" name="  c4   "/>
+    <tableColumn id="18" xr3:uid="{1721F398-E591-4221-9E97-CBB43E5CCD2A}" name="  c8   "/>
+    <tableColumn id="19" xr3:uid="{88A4285F-54BB-436F-A881-5B57A4F123C8}" name="  cq8  "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4700,7 +4877,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{338965B1-70E8-4C6E-9B36-81CFD9B4B68C}" name="Tableau2" displayName="Tableau2" ref="A38:M86" totalsRowShown="0">
   <autoFilter ref="A38:M86" xr:uid="{96ED0AB2-A97A-4D42-920C-6630AA3F4A02}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A0A5A8FD-7607-48B6-9135-5D249D0BCE0F}" name="Date       " dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{A0A5A8FD-7607-48B6-9135-5D249D0BCE0F}" name="Date       " dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{E51B31D0-A0A3-4931-B875-C0BC5FD9B82D}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{C80B30D5-1BC2-4F07-B77C-972433CC014E}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{DA26DA73-82A9-49AC-BEE0-07CB81D8E66E}" name=" Team2             "/>
@@ -4753,7 +4930,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A086498-695C-4792-B6A7-E6FA4AFD559A}" name="Tableau3" displayName="Tableau3" ref="A35:O83" totalsRowShown="0">
   <autoFilter ref="A35:O83" xr:uid="{A597B673-D5D6-41BB-8418-616CAD672A6C}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{28A461B9-B55B-45C3-A1C5-A72B63C0DE95}" name="Date       " dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{28A461B9-B55B-45C3-A1C5-A72B63C0DE95}" name="Date       " dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{4337CFE4-4E9E-483E-AB8D-9DE67C36B0A1}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{2182342D-CBD2-49C5-A25F-0F9C3CCD7107}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{85A22FCF-209F-43C5-A3D9-ABD31B6B3953}" name=" Team2             "/>
@@ -4809,7 +4986,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6945C8BF-54A5-4025-8EA4-289C7FB8B708}" name="Tableau6" displayName="Tableau6" ref="A71:P119" totalsRowShown="0">
   <autoFilter ref="A71:P119" xr:uid="{9830D998-6315-4F2D-A674-5B740BF3E00C}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{6632B7A1-23F7-4D06-A323-51A64A023F48}" name="Date       " dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{6632B7A1-23F7-4D06-A323-51A64A023F48}" name="Date       " dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{20A74076-22FE-423D-8C0C-581C372EB016}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{A20C27C7-B5D8-4DF8-BD6B-E977DF554B7D}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{F6FA5282-0C3B-4F38-93DE-4B7D0CC8DA41}" name=" Team2             "/>
@@ -7199,8 +7376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B268D9CD-BC4B-41C5-89D4-04A07034CAFF}">
   <dimension ref="A1:S82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10646,6 +10823,2721 @@
       </c>
       <c r="E82" t="s">
         <v>1391</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B031F157-2DBE-47F4-B3F1-B2831B36E5C8}">
+  <dimension ref="A1:S68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>1752</v>
+      </c>
+      <c r="C2">
+        <v>922</v>
+      </c>
+      <c r="D2">
+        <v>2784</v>
+      </c>
+      <c r="E2">
+        <v>4167</v>
+      </c>
+      <c r="F2">
+        <v>6255</v>
+      </c>
+      <c r="G2">
+        <v>9131</v>
+      </c>
+      <c r="H2">
+        <v>17.5</v>
+      </c>
+      <c r="I2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J2">
+        <v>27.8</v>
+      </c>
+      <c r="K2">
+        <v>41.7</v>
+      </c>
+      <c r="L2">
+        <v>62.5</v>
+      </c>
+      <c r="M2">
+        <v>91.3</v>
+      </c>
+      <c r="N2">
+        <v>5.7</v>
+      </c>
+      <c r="O2">
+        <v>10.8</v>
+      </c>
+      <c r="P2">
+        <v>3.6</v>
+      </c>
+      <c r="Q2">
+        <v>2.4</v>
+      </c>
+      <c r="R2">
+        <v>1.6</v>
+      </c>
+      <c r="S2">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>1543</v>
+      </c>
+      <c r="C3">
+        <v>1005</v>
+      </c>
+      <c r="D3">
+        <v>2926</v>
+      </c>
+      <c r="E3">
+        <v>4706</v>
+      </c>
+      <c r="F3">
+        <v>7631</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
+      </c>
+      <c r="H3">
+        <v>15.4</v>
+      </c>
+      <c r="I3">
+        <v>10.1</v>
+      </c>
+      <c r="J3">
+        <v>29.3</v>
+      </c>
+      <c r="K3">
+        <v>47.1</v>
+      </c>
+      <c r="L3">
+        <v>76.3</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>6.5</v>
+      </c>
+      <c r="O3">
+        <v>10</v>
+      </c>
+      <c r="P3">
+        <v>3.4</v>
+      </c>
+      <c r="Q3">
+        <v>2.1</v>
+      </c>
+      <c r="R3">
+        <v>1.3</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>930</v>
+      </c>
+      <c r="C4">
+        <v>860</v>
+      </c>
+      <c r="D4">
+        <v>1947</v>
+      </c>
+      <c r="E4">
+        <v>3665</v>
+      </c>
+      <c r="F4">
+        <v>6558</v>
+      </c>
+      <c r="G4">
+        <v>10000</v>
+      </c>
+      <c r="H4">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="I4">
+        <v>8.6</v>
+      </c>
+      <c r="J4">
+        <v>19.5</v>
+      </c>
+      <c r="K4">
+        <v>36.6</v>
+      </c>
+      <c r="L4">
+        <v>65.599999999999994</v>
+      </c>
+      <c r="M4">
+        <v>100</v>
+      </c>
+      <c r="N4">
+        <v>10.8</v>
+      </c>
+      <c r="O4">
+        <v>11.6</v>
+      </c>
+      <c r="P4">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="Q4">
+        <v>2.7</v>
+      </c>
+      <c r="R4">
+        <v>1.5</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>817</v>
+      </c>
+      <c r="C5">
+        <v>912</v>
+      </c>
+      <c r="D5">
+        <v>1585</v>
+      </c>
+      <c r="E5">
+        <v>3324</v>
+      </c>
+      <c r="F5">
+        <v>6953</v>
+      </c>
+      <c r="G5">
+        <v>10000</v>
+      </c>
+      <c r="H5">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I5">
+        <v>9.1</v>
+      </c>
+      <c r="J5">
+        <v>15.8</v>
+      </c>
+      <c r="K5">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="L5">
+        <v>69.5</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <v>12.2</v>
+      </c>
+      <c r="O5">
+        <v>11</v>
+      </c>
+      <c r="P5">
+        <v>6.3</v>
+      </c>
+      <c r="Q5">
+        <v>3</v>
+      </c>
+      <c r="R5">
+        <v>1.4</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>815</v>
+      </c>
+      <c r="C6">
+        <v>550</v>
+      </c>
+      <c r="D6">
+        <v>1370</v>
+      </c>
+      <c r="E6">
+        <v>2270</v>
+      </c>
+      <c r="F6">
+        <v>3678</v>
+      </c>
+      <c r="G6">
+        <v>7667</v>
+      </c>
+      <c r="H6">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I6">
+        <v>5.5</v>
+      </c>
+      <c r="J6">
+        <v>13.7</v>
+      </c>
+      <c r="K6">
+        <v>22.7</v>
+      </c>
+      <c r="L6">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="M6">
+        <v>76.7</v>
+      </c>
+      <c r="N6">
+        <v>12.3</v>
+      </c>
+      <c r="O6">
+        <v>18.2</v>
+      </c>
+      <c r="P6">
+        <v>7.3</v>
+      </c>
+      <c r="Q6">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R6">
+        <v>2.7</v>
+      </c>
+      <c r="S6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>800</v>
+      </c>
+      <c r="C7">
+        <v>931</v>
+      </c>
+      <c r="D7">
+        <v>1579</v>
+      </c>
+      <c r="E7">
+        <v>3268</v>
+      </c>
+      <c r="F7">
+        <v>7215</v>
+      </c>
+      <c r="G7">
+        <v>10000</v>
+      </c>
+      <c r="H7">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="J7">
+        <v>15.8</v>
+      </c>
+      <c r="K7">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="L7">
+        <v>72.2</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+      <c r="N7">
+        <v>12.5</v>
+      </c>
+      <c r="O7">
+        <v>10.7</v>
+      </c>
+      <c r="P7">
+        <v>6.3</v>
+      </c>
+      <c r="Q7">
+        <v>3.1</v>
+      </c>
+      <c r="R7">
+        <v>1.4</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>785</v>
+      </c>
+      <c r="C8">
+        <v>718</v>
+      </c>
+      <c r="D8">
+        <v>1683</v>
+      </c>
+      <c r="E8">
+        <v>3183</v>
+      </c>
+      <c r="F8">
+        <v>6472</v>
+      </c>
+      <c r="G8">
+        <v>10000</v>
+      </c>
+      <c r="H8">
+        <v>7.8</v>
+      </c>
+      <c r="I8">
+        <v>7.2</v>
+      </c>
+      <c r="J8">
+        <v>16.8</v>
+      </c>
+      <c r="K8">
+        <v>31.8</v>
+      </c>
+      <c r="L8">
+        <v>64.7</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+      <c r="N8">
+        <v>12.7</v>
+      </c>
+      <c r="O8">
+        <v>13.9</v>
+      </c>
+      <c r="P8">
+        <v>5.9</v>
+      </c>
+      <c r="Q8">
+        <v>3.1</v>
+      </c>
+      <c r="R8">
+        <v>1.5</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>559</v>
+      </c>
+      <c r="C9">
+        <v>736</v>
+      </c>
+      <c r="D9">
+        <v>1316</v>
+      </c>
+      <c r="E9">
+        <v>2813</v>
+      </c>
+      <c r="F9">
+        <v>5226</v>
+      </c>
+      <c r="G9">
+        <v>7861</v>
+      </c>
+      <c r="H9">
+        <v>5.6</v>
+      </c>
+      <c r="I9">
+        <v>7.4</v>
+      </c>
+      <c r="J9">
+        <v>13.2</v>
+      </c>
+      <c r="K9">
+        <v>28.1</v>
+      </c>
+      <c r="L9">
+        <v>52.3</v>
+      </c>
+      <c r="M9">
+        <v>78.599999999999994</v>
+      </c>
+      <c r="N9">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O9">
+        <v>13.6</v>
+      </c>
+      <c r="P9">
+        <v>7.6</v>
+      </c>
+      <c r="Q9">
+        <v>3.6</v>
+      </c>
+      <c r="R9">
+        <v>1.9</v>
+      </c>
+      <c r="S9">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10">
+        <v>439</v>
+      </c>
+      <c r="C10">
+        <v>738</v>
+      </c>
+      <c r="D10">
+        <v>902</v>
+      </c>
+      <c r="E10">
+        <v>2322</v>
+      </c>
+      <c r="F10">
+        <v>4655</v>
+      </c>
+      <c r="G10">
+        <v>9582</v>
+      </c>
+      <c r="H10">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I10">
+        <v>7.4</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>23.2</v>
+      </c>
+      <c r="L10">
+        <v>46.6</v>
+      </c>
+      <c r="M10">
+        <v>95.8</v>
+      </c>
+      <c r="N10">
+        <v>22.8</v>
+      </c>
+      <c r="O10">
+        <v>13.6</v>
+      </c>
+      <c r="P10">
+        <v>11.1</v>
+      </c>
+      <c r="Q10">
+        <v>4.3</v>
+      </c>
+      <c r="R10">
+        <v>2.1</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>403</v>
+      </c>
+      <c r="C11">
+        <v>643</v>
+      </c>
+      <c r="D11">
+        <v>856</v>
+      </c>
+      <c r="E11">
+        <v>2180</v>
+      </c>
+      <c r="F11">
+        <v>4263</v>
+      </c>
+      <c r="G11">
+        <v>9331</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>6.4</v>
+      </c>
+      <c r="J11">
+        <v>8.6</v>
+      </c>
+      <c r="K11">
+        <v>21.8</v>
+      </c>
+      <c r="L11">
+        <v>42.6</v>
+      </c>
+      <c r="M11">
+        <v>93.3</v>
+      </c>
+      <c r="N11">
+        <v>24.8</v>
+      </c>
+      <c r="O11">
+        <v>15.6</v>
+      </c>
+      <c r="P11">
+        <v>11.7</v>
+      </c>
+      <c r="Q11">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S11">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>285</v>
+      </c>
+      <c r="C12">
+        <v>366</v>
+      </c>
+      <c r="D12">
+        <v>597</v>
+      </c>
+      <c r="E12">
+        <v>1318</v>
+      </c>
+      <c r="F12">
+        <v>2951</v>
+      </c>
+      <c r="G12">
+        <v>6621</v>
+      </c>
+      <c r="H12">
+        <v>2.9</v>
+      </c>
+      <c r="I12">
+        <v>3.7</v>
+      </c>
+      <c r="J12">
+        <v>6</v>
+      </c>
+      <c r="K12">
+        <v>13.2</v>
+      </c>
+      <c r="L12">
+        <v>29.5</v>
+      </c>
+      <c r="M12">
+        <v>66.2</v>
+      </c>
+      <c r="N12">
+        <v>35.1</v>
+      </c>
+      <c r="O12">
+        <v>27.3</v>
+      </c>
+      <c r="P12">
+        <v>16.8</v>
+      </c>
+      <c r="Q12">
+        <v>7.6</v>
+      </c>
+      <c r="R12">
+        <v>3.4</v>
+      </c>
+      <c r="S12">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>213</v>
+      </c>
+      <c r="C13">
+        <v>257</v>
+      </c>
+      <c r="D13">
+        <v>521</v>
+      </c>
+      <c r="E13">
+        <v>1215</v>
+      </c>
+      <c r="F13">
+        <v>3052</v>
+      </c>
+      <c r="G13">
+        <v>10000</v>
+      </c>
+      <c r="H13">
+        <v>2.1</v>
+      </c>
+      <c r="I13">
+        <v>2.6</v>
+      </c>
+      <c r="J13">
+        <v>5.2</v>
+      </c>
+      <c r="K13">
+        <v>12.2</v>
+      </c>
+      <c r="L13">
+        <v>30.5</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13">
+        <v>46.9</v>
+      </c>
+      <c r="O13">
+        <v>38.9</v>
+      </c>
+      <c r="P13">
+        <v>19.2</v>
+      </c>
+      <c r="Q13">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="R13">
+        <v>3.3</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14">
+        <v>190</v>
+      </c>
+      <c r="C14">
+        <v>322</v>
+      </c>
+      <c r="D14">
+        <v>565</v>
+      </c>
+      <c r="E14">
+        <v>1429</v>
+      </c>
+      <c r="F14">
+        <v>3504</v>
+      </c>
+      <c r="G14">
+        <v>8540</v>
+      </c>
+      <c r="H14">
+        <v>1.9</v>
+      </c>
+      <c r="I14">
+        <v>3.2</v>
+      </c>
+      <c r="J14">
+        <v>5.7</v>
+      </c>
+      <c r="K14">
+        <v>14.3</v>
+      </c>
+      <c r="L14">
+        <v>35</v>
+      </c>
+      <c r="M14">
+        <v>85.4</v>
+      </c>
+      <c r="N14">
+        <v>52.6</v>
+      </c>
+      <c r="O14">
+        <v>31.1</v>
+      </c>
+      <c r="P14">
+        <v>17.7</v>
+      </c>
+      <c r="Q14">
+        <v>7</v>
+      </c>
+      <c r="R14">
+        <v>2.9</v>
+      </c>
+      <c r="S14">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>155</v>
+      </c>
+      <c r="C15">
+        <v>301</v>
+      </c>
+      <c r="D15">
+        <v>449</v>
+      </c>
+      <c r="E15">
+        <v>1223</v>
+      </c>
+      <c r="F15">
+        <v>3069</v>
+      </c>
+      <c r="G15">
+        <v>10000</v>
+      </c>
+      <c r="H15">
+        <v>1.6</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>4.5</v>
+      </c>
+      <c r="K15">
+        <v>12.2</v>
+      </c>
+      <c r="L15">
+        <v>30.7</v>
+      </c>
+      <c r="M15">
+        <v>100</v>
+      </c>
+      <c r="N15">
+        <v>64.5</v>
+      </c>
+      <c r="O15">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="P15">
+        <v>22.3</v>
+      </c>
+      <c r="Q15">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="R15">
+        <v>3.3</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>147</v>
+      </c>
+      <c r="C16">
+        <v>262</v>
+      </c>
+      <c r="D16">
+        <v>357</v>
+      </c>
+      <c r="E16">
+        <v>942</v>
+      </c>
+      <c r="F16">
+        <v>1972</v>
+      </c>
+      <c r="G16">
+        <v>5171</v>
+      </c>
+      <c r="H16">
+        <v>1.5</v>
+      </c>
+      <c r="I16">
+        <v>2.6</v>
+      </c>
+      <c r="J16">
+        <v>3.6</v>
+      </c>
+      <c r="K16">
+        <v>9.4</v>
+      </c>
+      <c r="L16">
+        <v>19.7</v>
+      </c>
+      <c r="M16">
+        <v>51.7</v>
+      </c>
+      <c r="N16">
+        <v>68</v>
+      </c>
+      <c r="O16">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="P16">
+        <v>28</v>
+      </c>
+      <c r="Q16">
+        <v>10.6</v>
+      </c>
+      <c r="R16">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="S16">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>41</v>
+      </c>
+      <c r="C17">
+        <v>98</v>
+      </c>
+      <c r="D17">
+        <v>98</v>
+      </c>
+      <c r="E17">
+        <v>382</v>
+      </c>
+      <c r="F17">
+        <v>1466</v>
+      </c>
+      <c r="G17">
+        <v>7124</v>
+      </c>
+      <c r="H17">
+        <v>0.4</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <v>3.8</v>
+      </c>
+      <c r="L17">
+        <v>14.7</v>
+      </c>
+      <c r="M17">
+        <v>71.2</v>
+      </c>
+      <c r="N17">
+        <v>243.9</v>
+      </c>
+      <c r="O17">
+        <v>102</v>
+      </c>
+      <c r="P17">
+        <v>102</v>
+      </c>
+      <c r="Q17">
+        <v>26.2</v>
+      </c>
+      <c r="R17">
+        <v>6.8</v>
+      </c>
+      <c r="S17">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>39</v>
+      </c>
+      <c r="C18">
+        <v>78</v>
+      </c>
+      <c r="D18">
+        <v>124</v>
+      </c>
+      <c r="E18">
+        <v>367</v>
+      </c>
+      <c r="F18">
+        <v>1022</v>
+      </c>
+      <c r="G18">
+        <v>2139</v>
+      </c>
+      <c r="H18">
+        <v>0.4</v>
+      </c>
+      <c r="I18">
+        <v>0.8</v>
+      </c>
+      <c r="J18">
+        <v>1.2</v>
+      </c>
+      <c r="K18">
+        <v>3.7</v>
+      </c>
+      <c r="L18">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="M18">
+        <v>21.4</v>
+      </c>
+      <c r="N18">
+        <v>256.39999999999998</v>
+      </c>
+      <c r="O18">
+        <v>128.19999999999999</v>
+      </c>
+      <c r="P18">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="Q18">
+        <v>27.2</v>
+      </c>
+      <c r="R18">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="S18">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>28</v>
+      </c>
+      <c r="C19">
+        <v>99</v>
+      </c>
+      <c r="D19">
+        <v>119</v>
+      </c>
+      <c r="E19">
+        <v>383</v>
+      </c>
+      <c r="F19">
+        <v>1415</v>
+      </c>
+      <c r="G19">
+        <v>6255</v>
+      </c>
+      <c r="H19">
+        <v>0.3</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1.2</v>
+      </c>
+      <c r="K19">
+        <v>3.8</v>
+      </c>
+      <c r="L19">
+        <v>14.1</v>
+      </c>
+      <c r="M19">
+        <v>62.5</v>
+      </c>
+      <c r="N19">
+        <v>357.1</v>
+      </c>
+      <c r="O19">
+        <v>101</v>
+      </c>
+      <c r="P19">
+        <v>84</v>
+      </c>
+      <c r="Q19">
+        <v>26.1</v>
+      </c>
+      <c r="R19">
+        <v>7.1</v>
+      </c>
+      <c r="S19">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>22</v>
+      </c>
+      <c r="C20">
+        <v>73</v>
+      </c>
+      <c r="D20">
+        <v>65</v>
+      </c>
+      <c r="E20">
+        <v>281</v>
+      </c>
+      <c r="F20">
+        <v>901</v>
+      </c>
+      <c r="G20">
+        <v>4186</v>
+      </c>
+      <c r="H20">
+        <v>0.2</v>
+      </c>
+      <c r="I20">
+        <v>0.7</v>
+      </c>
+      <c r="J20">
+        <v>0.7</v>
+      </c>
+      <c r="K20">
+        <v>2.8</v>
+      </c>
+      <c r="L20">
+        <v>9</v>
+      </c>
+      <c r="M20">
+        <v>41.9</v>
+      </c>
+      <c r="N20">
+        <v>454.5</v>
+      </c>
+      <c r="O20">
+        <v>137</v>
+      </c>
+      <c r="P20">
+        <v>153.80000000000001</v>
+      </c>
+      <c r="Q20">
+        <v>35.6</v>
+      </c>
+      <c r="R20">
+        <v>11.1</v>
+      </c>
+      <c r="S20">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>36</v>
+      </c>
+      <c r="D21">
+        <v>48</v>
+      </c>
+      <c r="E21">
+        <v>155</v>
+      </c>
+      <c r="F21">
+        <v>438</v>
+      </c>
+      <c r="G21">
+        <v>1287</v>
+      </c>
+      <c r="H21">
+        <v>0.1</v>
+      </c>
+      <c r="I21">
+        <v>0.4</v>
+      </c>
+      <c r="J21">
+        <v>0.5</v>
+      </c>
+      <c r="K21">
+        <v>1.6</v>
+      </c>
+      <c r="L21">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M21">
+        <v>12.9</v>
+      </c>
+      <c r="N21">
+        <v>769.2</v>
+      </c>
+      <c r="O21">
+        <v>277.8</v>
+      </c>
+      <c r="P21">
+        <v>208.3</v>
+      </c>
+      <c r="Q21">
+        <v>64.5</v>
+      </c>
+      <c r="R21">
+        <v>22.8</v>
+      </c>
+      <c r="S21">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>12</v>
+      </c>
+      <c r="C22">
+        <v>50</v>
+      </c>
+      <c r="D22">
+        <v>51</v>
+      </c>
+      <c r="E22">
+        <v>203</v>
+      </c>
+      <c r="F22">
+        <v>605</v>
+      </c>
+      <c r="G22">
+        <v>2352</v>
+      </c>
+      <c r="H22">
+        <v>0.1</v>
+      </c>
+      <c r="I22">
+        <v>0.5</v>
+      </c>
+      <c r="J22">
+        <v>0.5</v>
+      </c>
+      <c r="K22">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>6</v>
+      </c>
+      <c r="M22">
+        <v>23.5</v>
+      </c>
+      <c r="N22">
+        <v>833.3</v>
+      </c>
+      <c r="O22">
+        <v>200</v>
+      </c>
+      <c r="P22">
+        <v>196.1</v>
+      </c>
+      <c r="Q22">
+        <v>49.3</v>
+      </c>
+      <c r="R22">
+        <v>16.5</v>
+      </c>
+      <c r="S22">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>31</v>
+      </c>
+      <c r="D23">
+        <v>34</v>
+      </c>
+      <c r="E23">
+        <v>126</v>
+      </c>
+      <c r="F23">
+        <v>419</v>
+      </c>
+      <c r="G23">
+        <v>1460</v>
+      </c>
+      <c r="H23">
+        <v>0.1</v>
+      </c>
+      <c r="I23">
+        <v>0.3</v>
+      </c>
+      <c r="J23">
+        <v>0.3</v>
+      </c>
+      <c r="K23">
+        <v>1.3</v>
+      </c>
+      <c r="L23">
+        <v>4.2</v>
+      </c>
+      <c r="M23">
+        <v>14.6</v>
+      </c>
+      <c r="N23">
+        <v>1250</v>
+      </c>
+      <c r="O23">
+        <v>322.60000000000002</v>
+      </c>
+      <c r="P23">
+        <v>294.10000000000002</v>
+      </c>
+      <c r="Q23">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="R23">
+        <v>23.9</v>
+      </c>
+      <c r="S23">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>13</v>
+      </c>
+      <c r="E24">
+        <v>50</v>
+      </c>
+      <c r="F24">
+        <v>174</v>
+      </c>
+      <c r="G24">
+        <v>643</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0.1</v>
+      </c>
+      <c r="J24">
+        <v>0.1</v>
+      </c>
+      <c r="K24">
+        <v>0.5</v>
+      </c>
+      <c r="L24">
+        <v>1.7</v>
+      </c>
+      <c r="M24">
+        <v>6.4</v>
+      </c>
+      <c r="N24">
+        <v>3333.3</v>
+      </c>
+      <c r="O24">
+        <v>1000</v>
+      </c>
+      <c r="P24">
+        <v>769.2</v>
+      </c>
+      <c r="Q24">
+        <v>200</v>
+      </c>
+      <c r="R24">
+        <v>57.5</v>
+      </c>
+      <c r="S24">
+        <v>15.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+      <c r="D25">
+        <v>11</v>
+      </c>
+      <c r="E25">
+        <v>28</v>
+      </c>
+      <c r="F25">
+        <v>106</v>
+      </c>
+      <c r="G25">
+        <v>650</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0.1</v>
+      </c>
+      <c r="K25">
+        <v>0.3</v>
+      </c>
+      <c r="L25">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M25">
+        <v>6.5</v>
+      </c>
+      <c r="N25">
+        <v>10000</v>
+      </c>
+      <c r="O25">
+        <v>5000</v>
+      </c>
+      <c r="P25">
+        <v>909.1</v>
+      </c>
+      <c r="Q25">
+        <v>357.1</v>
+      </c>
+      <c r="R25">
+        <v>94.3</v>
+      </c>
+      <c r="S25">
+        <v>15.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" t="s">
+        <v>54</v>
+      </c>
+      <c r="E27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" t="s">
+        <v>56</v>
+      </c>
+      <c r="J27" t="s">
+        <v>41</v>
+      </c>
+      <c r="K27" t="s">
+        <v>45</v>
+      </c>
+      <c r="L27" t="s">
+        <v>57</v>
+      </c>
+      <c r="M27" t="s">
+        <v>58</v>
+      </c>
+      <c r="N27" t="s">
+        <v>255</v>
+      </c>
+      <c r="O27" t="s">
+        <v>256</v>
+      </c>
+      <c r="P27" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43276</v>
+      </c>
+      <c r="B28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C28" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28">
+        <v>2916</v>
+      </c>
+      <c r="F28">
+        <v>2140</v>
+      </c>
+      <c r="G28">
+        <v>4944</v>
+      </c>
+      <c r="H28">
+        <v>29.2</v>
+      </c>
+      <c r="I28">
+        <v>21.4</v>
+      </c>
+      <c r="J28">
+        <v>49.4</v>
+      </c>
+      <c r="K28">
+        <v>3.4</v>
+      </c>
+      <c r="L28">
+        <v>4.7</v>
+      </c>
+      <c r="M28">
+        <v>2</v>
+      </c>
+      <c r="N28">
+        <v>1.7</v>
+      </c>
+      <c r="O28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43276</v>
+      </c>
+      <c r="B29" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
+      </c>
+      <c r="D29" t="s">
+        <v>63</v>
+      </c>
+      <c r="E29">
+        <v>7681</v>
+      </c>
+      <c r="F29">
+        <v>1268</v>
+      </c>
+      <c r="G29">
+        <v>1051</v>
+      </c>
+      <c r="H29">
+        <v>76.8</v>
+      </c>
+      <c r="I29">
+        <v>12.7</v>
+      </c>
+      <c r="J29">
+        <v>10.5</v>
+      </c>
+      <c r="K29">
+        <v>1.3</v>
+      </c>
+      <c r="L29">
+        <v>7.9</v>
+      </c>
+      <c r="M29">
+        <v>9.5</v>
+      </c>
+      <c r="N29">
+        <v>2.6</v>
+      </c>
+      <c r="O29">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43276</v>
+      </c>
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30">
+        <v>2139</v>
+      </c>
+      <c r="F30">
+        <v>1849</v>
+      </c>
+      <c r="G30">
+        <v>6012</v>
+      </c>
+      <c r="H30">
+        <v>21.4</v>
+      </c>
+      <c r="I30">
+        <v>18.5</v>
+      </c>
+      <c r="J30">
+        <v>60.1</v>
+      </c>
+      <c r="K30">
+        <v>4.7</v>
+      </c>
+      <c r="L30">
+        <v>5.4</v>
+      </c>
+      <c r="M30">
+        <v>1.7</v>
+      </c>
+      <c r="N30">
+        <v>1.6</v>
+      </c>
+      <c r="O30">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43276</v>
+      </c>
+      <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31" t="s">
+        <v>60</v>
+      </c>
+      <c r="E31">
+        <v>4104</v>
+      </c>
+      <c r="F31">
+        <v>2144</v>
+      </c>
+      <c r="G31">
+        <v>3752</v>
+      </c>
+      <c r="H31">
+        <v>41</v>
+      </c>
+      <c r="I31">
+        <v>21.4</v>
+      </c>
+      <c r="J31">
+        <v>37.5</v>
+      </c>
+      <c r="K31">
+        <v>2.4</v>
+      </c>
+      <c r="L31">
+        <v>4.7</v>
+      </c>
+      <c r="M31">
+        <v>2.7</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>43277</v>
+      </c>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32">
+        <v>2364</v>
+      </c>
+      <c r="F32">
+        <v>1953</v>
+      </c>
+      <c r="G32">
+        <v>5683</v>
+      </c>
+      <c r="H32">
+        <v>23.6</v>
+      </c>
+      <c r="I32">
+        <v>19.5</v>
+      </c>
+      <c r="J32">
+        <v>56.8</v>
+      </c>
+      <c r="K32">
+        <v>4.2</v>
+      </c>
+      <c r="L32">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M32">
+        <v>1.8</v>
+      </c>
+      <c r="N32">
+        <v>1.7</v>
+      </c>
+      <c r="O32">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>43277</v>
+      </c>
+      <c r="B33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s">
+        <v>79</v>
+      </c>
+      <c r="D33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33">
+        <v>1685</v>
+      </c>
+      <c r="F33">
+        <v>1648</v>
+      </c>
+      <c r="G33">
+        <v>6667</v>
+      </c>
+      <c r="H33">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="I33">
+        <v>16.5</v>
+      </c>
+      <c r="J33">
+        <v>66.7</v>
+      </c>
+      <c r="K33">
+        <v>5.9</v>
+      </c>
+      <c r="L33">
+        <v>6.1</v>
+      </c>
+      <c r="M33">
+        <v>1.5</v>
+      </c>
+      <c r="N33">
+        <v>1.6</v>
+      </c>
+      <c r="O33">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>43277</v>
+      </c>
+      <c r="B34" t="s">
+        <v>129</v>
+      </c>
+      <c r="C34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34">
+        <v>2626</v>
+      </c>
+      <c r="F34">
+        <v>2017</v>
+      </c>
+      <c r="G34">
+        <v>5357</v>
+      </c>
+      <c r="H34">
+        <v>26.3</v>
+      </c>
+      <c r="I34">
+        <v>20.2</v>
+      </c>
+      <c r="J34">
+        <v>53.6</v>
+      </c>
+      <c r="K34">
+        <v>3.8</v>
+      </c>
+      <c r="L34">
+        <v>5</v>
+      </c>
+      <c r="M34">
+        <v>1.9</v>
+      </c>
+      <c r="N34">
+        <v>1.7</v>
+      </c>
+      <c r="O34">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>43277</v>
+      </c>
+      <c r="B35" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35">
+        <v>2738</v>
+      </c>
+      <c r="F35">
+        <v>2113</v>
+      </c>
+      <c r="G35">
+        <v>5149</v>
+      </c>
+      <c r="H35">
+        <v>27.4</v>
+      </c>
+      <c r="I35">
+        <v>21.1</v>
+      </c>
+      <c r="J35">
+        <v>51.5</v>
+      </c>
+      <c r="K35">
+        <v>3.7</v>
+      </c>
+      <c r="L35">
+        <v>4.7</v>
+      </c>
+      <c r="M35">
+        <v>1.9</v>
+      </c>
+      <c r="N35">
+        <v>1.8</v>
+      </c>
+      <c r="O35">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>43278</v>
+      </c>
+      <c r="B36" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" t="s">
+        <v>90</v>
+      </c>
+      <c r="E36">
+        <v>1056</v>
+      </c>
+      <c r="F36">
+        <v>1334</v>
+      </c>
+      <c r="G36">
+        <v>7610</v>
+      </c>
+      <c r="H36">
+        <v>10.6</v>
+      </c>
+      <c r="I36">
+        <v>13.3</v>
+      </c>
+      <c r="J36">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="K36">
+        <v>9.5</v>
+      </c>
+      <c r="L36">
+        <v>7.5</v>
+      </c>
+      <c r="M36">
+        <v>1.3</v>
+      </c>
+      <c r="N36">
+        <v>1.5</v>
+      </c>
+      <c r="O36">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>43278</v>
+      </c>
+      <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37">
+        <v>6487</v>
+      </c>
+      <c r="F37">
+        <v>1737</v>
+      </c>
+      <c r="G37">
+        <v>1776</v>
+      </c>
+      <c r="H37">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="I37">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="J37">
+        <v>17.8</v>
+      </c>
+      <c r="K37">
+        <v>1.5</v>
+      </c>
+      <c r="L37">
+        <v>5.8</v>
+      </c>
+      <c r="M37">
+        <v>5.6</v>
+      </c>
+      <c r="N37">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O37">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>43278</v>
+      </c>
+      <c r="B38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>84</v>
+      </c>
+      <c r="E38">
+        <v>1216</v>
+      </c>
+      <c r="F38">
+        <v>1387</v>
+      </c>
+      <c r="G38">
+        <v>7397</v>
+      </c>
+      <c r="H38">
+        <v>12.2</v>
+      </c>
+      <c r="I38">
+        <v>13.9</v>
+      </c>
+      <c r="J38">
+        <v>74</v>
+      </c>
+      <c r="K38">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L38">
+        <v>7.2</v>
+      </c>
+      <c r="M38">
+        <v>1.4</v>
+      </c>
+      <c r="N38">
+        <v>1.6</v>
+      </c>
+      <c r="O38">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43278</v>
+      </c>
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39">
+        <v>5419</v>
+      </c>
+      <c r="F39">
+        <v>1978</v>
+      </c>
+      <c r="G39">
+        <v>2603</v>
+      </c>
+      <c r="H39">
+        <v>54.2</v>
+      </c>
+      <c r="I39">
+        <v>19.8</v>
+      </c>
+      <c r="J39">
+        <v>26</v>
+      </c>
+      <c r="K39">
+        <v>1.8</v>
+      </c>
+      <c r="L39">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M39">
+        <v>3.8</v>
+      </c>
+      <c r="N39">
+        <v>2.1</v>
+      </c>
+      <c r="O39">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43279</v>
+      </c>
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D40" t="s">
+        <v>99</v>
+      </c>
+      <c r="E40">
+        <v>3758</v>
+      </c>
+      <c r="F40">
+        <v>2225</v>
+      </c>
+      <c r="G40">
+        <v>4017</v>
+      </c>
+      <c r="H40">
+        <v>37.6</v>
+      </c>
+      <c r="I40">
+        <v>22.2</v>
+      </c>
+      <c r="J40">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="K40">
+        <v>2.7</v>
+      </c>
+      <c r="L40">
+        <v>4.5</v>
+      </c>
+      <c r="M40">
+        <v>2.5</v>
+      </c>
+      <c r="N40">
+        <v>1.8</v>
+      </c>
+      <c r="O40">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>43279</v>
+      </c>
+      <c r="B41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41">
+        <v>2154</v>
+      </c>
+      <c r="F41">
+        <v>1942</v>
+      </c>
+      <c r="G41">
+        <v>5904</v>
+      </c>
+      <c r="H41">
+        <v>21.5</v>
+      </c>
+      <c r="I41">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="J41">
+        <v>59</v>
+      </c>
+      <c r="K41">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L41">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M41">
+        <v>1.7</v>
+      </c>
+      <c r="N41">
+        <v>1.7</v>
+      </c>
+      <c r="O41">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43279</v>
+      </c>
+      <c r="B42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D42" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42">
+        <v>4268</v>
+      </c>
+      <c r="F42">
+        <v>2100</v>
+      </c>
+      <c r="G42">
+        <v>3632</v>
+      </c>
+      <c r="H42">
+        <v>42.7</v>
+      </c>
+      <c r="I42">
+        <v>21</v>
+      </c>
+      <c r="J42">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="K42">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L42">
+        <v>4.8</v>
+      </c>
+      <c r="M42">
+        <v>2.8</v>
+      </c>
+      <c r="N42">
+        <v>1.9</v>
+      </c>
+      <c r="O42">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43279</v>
+      </c>
+      <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
+        <v>100</v>
+      </c>
+      <c r="D43" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43">
+        <v>2807</v>
+      </c>
+      <c r="F43">
+        <v>2084</v>
+      </c>
+      <c r="G43">
+        <v>5109</v>
+      </c>
+      <c r="H43">
+        <v>28.1</v>
+      </c>
+      <c r="I43">
+        <v>20.8</v>
+      </c>
+      <c r="J43">
+        <v>51.1</v>
+      </c>
+      <c r="K43">
+        <v>3.6</v>
+      </c>
+      <c r="L43">
+        <v>4.8</v>
+      </c>
+      <c r="M43">
+        <v>2</v>
+      </c>
+      <c r="N43">
+        <v>1.7</v>
+      </c>
+      <c r="O43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B45" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1394</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C47" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1393</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" t="s">
+        <v>159</v>
+      </c>
+      <c r="E48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C49" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1396</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1397</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B50" t="s">
+        <v>1398</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D50" t="s">
+        <v>1399</v>
+      </c>
+      <c r="E50" t="s">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" t="s">
+        <v>163</v>
+      </c>
+      <c r="D51" t="s">
+        <v>164</v>
+      </c>
+      <c r="E51" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B52" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1401</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E52" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B53" t="s">
+        <v>1403</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1404</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1401</v>
+      </c>
+      <c r="E53" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B54" t="s">
+        <v>167</v>
+      </c>
+      <c r="C54" t="s">
+        <v>168</v>
+      </c>
+      <c r="D54" t="s">
+        <v>169</v>
+      </c>
+      <c r="E54" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1405</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E55" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B56" t="s">
+        <v>1407</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1406</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1408</v>
+      </c>
+      <c r="E56" t="s">
+        <v>1409</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B57" t="s">
+        <v>172</v>
+      </c>
+      <c r="C57" t="s">
+        <v>173</v>
+      </c>
+      <c r="D57" t="s">
+        <v>174</v>
+      </c>
+      <c r="E57" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B58" t="s">
+        <v>1410</v>
+      </c>
+      <c r="C58" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1411</v>
+      </c>
+      <c r="E58" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1413</v>
+      </c>
+      <c r="C59" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1414</v>
+      </c>
+      <c r="E59" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B60" t="s">
+        <v>177</v>
+      </c>
+      <c r="C60" t="s">
+        <v>178</v>
+      </c>
+      <c r="D60" t="s">
+        <v>179</v>
+      </c>
+      <c r="E60" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C61" t="s">
+        <v>1392</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1417</v>
+      </c>
+      <c r="E61" t="s">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C62" t="s">
+        <v>1420</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1421</v>
+      </c>
+      <c r="E62" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B63" t="s">
+        <v>182</v>
+      </c>
+      <c r="C63" t="s">
+        <v>183</v>
+      </c>
+      <c r="D63" t="s">
+        <v>184</v>
+      </c>
+      <c r="E63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B64" t="s">
+        <v>1423</v>
+      </c>
+      <c r="C64" t="s">
+        <v>1424</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E64" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B65" t="s">
+        <v>1424</v>
+      </c>
+      <c r="C65" t="s">
+        <v>1423</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E65" t="s">
+        <v>1392</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" t="s">
+        <v>187</v>
+      </c>
+      <c r="C66" t="s">
+        <v>188</v>
+      </c>
+      <c r="D66" t="s">
+        <v>189</v>
+      </c>
+      <c r="E66" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B67" t="s">
+        <v>1425</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E67" t="s">
+        <v>1427</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B68" t="s">
+        <v>1428</v>
+      </c>
+      <c r="C68" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E68" t="s">
+        <v>1430</v>
       </c>
     </row>
   </sheetData>
@@ -16684,8 +19576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EDCC70E-4B25-4A02-BEF5-B30B1429A772}">
   <dimension ref="A1:S143"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Mise à jour à la fin des matchs de poules
</commit_message>
<xml_diff>
--- a/Results_20180606.xlsx
+++ b/Results_20180606.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dompd\Document\worldcup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC63D4B-3BC9-492B-BC3B-DD5DA0E6F08B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F3FE56-405F-49E0-BF7C-073D7894C5C2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="6570" tabRatio="747" activeTab="10" xr2:uid="{E93A372B-1490-4A28-B29E-3CD0AFC460B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18405" windowHeight="6570" tabRatio="747" firstSheet="2" activeTab="11" xr2:uid="{E93A372B-1490-4A28-B29E-3CD0AFC460B9}"/>
   </bookViews>
   <sheets>
     <sheet name="GivenZeroEloNewProbaNumpyF" sheetId="13" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="20180621" sheetId="20" r:id="rId9"/>
     <sheet name="20180623" sheetId="21" r:id="rId10"/>
     <sheet name="20180624" sheetId="22" r:id="rId11"/>
+    <sheet name="20180629" sheetId="23" r:id="rId12"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5734" uniqueCount="1431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5808" uniqueCount="1439">
   <si>
     <t xml:space="preserve"> 1M  </t>
   </si>
@@ -4328,6 +4329,30 @@
   </si>
   <si>
     <t xml:space="preserve"> 3340   33   3,0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8AB     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8CD     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8BA     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8DC     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8EF     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8GH     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8FE     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8HG     </t>
   </si>
 </sst>
 </file>
@@ -4412,7 +4437,10 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
@@ -4492,7 +4520,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{9347FB5C-412B-40E4-B41C-02A6FE0AE109}" name="Tableau8" displayName="Tableau8" ref="A35:P83" totalsRowShown="0">
   <autoFilter ref="A35:P83" xr:uid="{EDDAA4B0-4193-4019-AE5F-84EBF522F9B7}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{43B17E18-2CA7-4710-A569-99665BF192B8}" name="Date       " dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{43B17E18-2CA7-4710-A569-99665BF192B8}" name="Date       " dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{18B91E56-AB03-41DF-8AA6-39846E8A232D}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{61520696-7ABA-491A-B0E9-DC64F7B4D675}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{DAF25AD3-8A89-40EA-9E2E-304087E594D0}" name=" Team2             "/>
@@ -4564,7 +4592,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7C38957E-D3C3-4EDE-8C2B-17F0C9D00713}" name="Tableau13" displayName="Tableau13" ref="A35:P83" totalsRowShown="0">
   <autoFilter ref="A35:P83" xr:uid="{0D6341F4-3D48-495C-9EA8-AE26D5F92808}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{51876778-EE60-4DB5-807C-3BAF31F3EBA7}" name="Date       " dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{51876778-EE60-4DB5-807C-3BAF31F3EBA7}" name="Date       " dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{355B6899-F63D-4BB3-AC20-86507223A1DE}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{5B238E8D-5A42-4AA8-8DDA-0E8C007BEA13}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{7415F0D1-2339-4094-B4CA-DA1E67C3B8EA}" name=" Team2             "/>
@@ -4634,7 +4662,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{CE74AF0B-2793-4D5F-AB14-98A0B7A5496B}" name="Tableau16" displayName="Tableau16" ref="A35:O67" totalsRowShown="0">
   <autoFilter ref="A35:O67" xr:uid="{69E73736-E9F1-4F73-A95D-947FCB875A43}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{0392F536-43A6-4135-BEBC-512373D21627}" name="Date       " dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{0392F536-43A6-4135-BEBC-512373D21627}" name="Date       " dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{7BAB4429-37F6-4193-A8F8-F41D34E505D6}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{3B193FBE-751B-4A4F-93E2-DF4A408FB3D8}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{6284F227-005C-4A09-AA27-A79FD219F58E}" name=" Team2             "/>
@@ -4689,7 +4717,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{F69BDF94-37F3-4256-A51D-135B8671BBA5}" name="Tableau18" displayName="Tableau18" ref="A35:O60" totalsRowShown="0">
   <autoFilter ref="A35:O60" xr:uid="{C72E9688-1DB9-4326-AAFD-05173885C691}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{3CBB2762-D6F0-4569-9979-8C76659F6CC5}" name="Date       " dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{3CBB2762-D6F0-4569-9979-8C76659F6CC5}" name="Date       " dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{BFA086CA-AE8D-4E23-AC75-DD0FDDD097DA}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{3F61DBAB-FA0F-4F11-A4D7-7FA6D75A7595}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{E27010C3-F9B7-4499-A5E2-1EC7EB737B35}" name=" Team2             "/>
@@ -4744,7 +4772,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{0D407DA2-1E3C-4BF9-9DEE-6FB85EA50B45}" name="Tableau11" displayName="Tableau11" ref="A1:M49" totalsRowShown="0">
   <autoFilter ref="A1:M49" xr:uid="{23AFB364-C990-4A52-88E8-7FFEF3078878}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{715799BB-9DC7-47F7-B86F-82ABC24CB807}" name="Date       " dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{715799BB-9DC7-47F7-B86F-82ABC24CB807}" name="Date       " dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{4203B992-4E6D-4429-85EA-C12615438D81}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{BFDE9085-79AD-4E69-824A-7F37EFD0712D}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{C450FEF0-7D71-4ABC-98B4-BB1C92D77557}" name=" Team2             "/>
@@ -4766,7 +4794,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{A8D74ED4-D634-440E-B79D-A0CECB3D0BB4}" name="Tableau20" displayName="Tableau20" ref="A35:O57" totalsRowShown="0">
   <autoFilter ref="A35:O57" xr:uid="{DBC3BA96-1AEA-4E50-8EFB-3B8F2A65E034}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{505A2FAA-9C6E-4FAA-AFF9-AEB929DD9CC6}" name="Date       " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{505A2FAA-9C6E-4FAA-AFF9-AEB929DD9CC6}" name="Date       " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{867A407D-4178-4402-A799-18F5A03E371D}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{7861AA1D-8038-4664-9ADF-6B396876114D}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{55DE77B8-DAE3-4901-9AB5-4C62EB2FDE99}" name=" Team2             "/>
@@ -4790,7 +4818,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{7089D5EB-82AB-4559-BE4B-61E1D3CA6A63}" name="Tableau22" displayName="Tableau22" ref="A27:P43" totalsRowShown="0">
   <autoFilter ref="A27:P43" xr:uid="{524D6DE2-B53E-4BBA-8981-8113AD62C0B8}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{9C67B6D3-D448-4651-BD7D-389542AC0269}" name="Date       " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9C67B6D3-D448-4651-BD7D-389542AC0269}" name="Date       " dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{3B559211-2D70-475D-8EA0-7AC81A7824E8}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{37269AF9-F2D2-4764-A769-81F3DE821B5F}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{EF245AAD-278C-436F-B4BE-1841C2C25E47}" name=" Team2             "/>
@@ -4842,6 +4870,61 @@
 </table>
 </file>
 
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{08890BF0-A9A4-4B4C-92FF-B9E956C44F95}" name="Tableau23" displayName="Tableau23" ref="A1:S17" totalsRowShown="0">
+  <autoFilter ref="A1:S17" xr:uid="{A3FCC47F-959B-43A2-8EF8-B04206353001}"/>
+  <sortState ref="A2:S17">
+    <sortCondition descending="1" ref="B1:B17"/>
+  </sortState>
+  <tableColumns count="19">
+    <tableColumn id="1" xr3:uid="{16632793-3DFF-4B01-8B81-4EBA9343A5AD}" name="       Teams        "/>
+    <tableColumn id="2" xr3:uid="{E2A39F46-88AE-4E76-9A4A-F2A017C3FF6B}" name="1"/>
+    <tableColumn id="3" xr3:uid="{DED0098F-02A0-403D-B7D4-00FF6D49EACE}" name=" 1M  "/>
+    <tableColumn id="4" xr3:uid="{B0A30BE9-ECA8-47C4-8D4B-1B5D71DC7E05}" name="2"/>
+    <tableColumn id="5" xr3:uid="{F93320A0-293F-461C-8869-AB932D5033EA}" name="4"/>
+    <tableColumn id="6" xr3:uid="{E1480EF9-AD19-4FDC-A5CE-69F045292548}" name="8"/>
+    <tableColumn id="7" xr3:uid="{30E6A521-3A5B-406B-836E-B9DCE60CAA72}" name=" q8  "/>
+    <tableColumn id="8" xr3:uid="{E9F107CB-5BE9-42B0-BC95-A4A2A32AE9A2}" name="  p1   "/>
+    <tableColumn id="9" xr3:uid="{5DD64BBA-D3DC-4E23-B185-A9FEE78956F9}" name="  p1M  "/>
+    <tableColumn id="10" xr3:uid="{F7DDDB5B-CD76-4F13-8B3B-6492C147D110}" name="  p2   "/>
+    <tableColumn id="11" xr3:uid="{5C9F5AC6-C928-4CA9-BBA7-ECCA5D1BFA48}" name="  p4   "/>
+    <tableColumn id="12" xr3:uid="{6B1FB922-C4D7-4B25-B822-7AC396283D82}" name="  p8   "/>
+    <tableColumn id="13" xr3:uid="{8CCB57D3-EF97-4967-9858-2665ECAC7A26}" name="  pq8  "/>
+    <tableColumn id="14" xr3:uid="{3B230983-DF03-4D0D-9512-B71E9CF5B122}" name="  c1   "/>
+    <tableColumn id="15" xr3:uid="{A6EA9E88-2E2D-4248-86D5-C22E7E13CBDB}" name="  c1M  "/>
+    <tableColumn id="16" xr3:uid="{5D6793DE-60DB-431F-B02F-DBC65C8B9D65}" name="  c2   "/>
+    <tableColumn id="17" xr3:uid="{C31859EA-F1AF-466E-9A82-0B8EE86E40F2}" name="  c4   "/>
+    <tableColumn id="18" xr3:uid="{69143E82-2DC9-44D3-B8B9-0F01937782AB}" name="  c8   "/>
+    <tableColumn id="19" xr3:uid="{033DC7C8-A18A-4FC8-82F8-AC1455580471}" name="  cq8  "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="24" xr:uid="{1F4BD138-C3B9-4DE9-99D6-F3E36AA4ED70}" name="Tableau24" displayName="Tableau24" ref="A20:O28" totalsRowShown="0">
+  <autoFilter ref="A20:O28" xr:uid="{91AC6D7C-E3C7-4796-A125-70A0C85BD91A}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{4E49A154-D696-402F-AE3C-78783217CB8F}" name="Date       " dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{44A7648A-2AD5-4BA1-89CF-BBC425B26306}" name="    Code    "/>
+    <tableColumn id="3" xr3:uid="{2F3E419C-DD24-4FA6-A9AD-1B8DCC533154}" name=" Team1             "/>
+    <tableColumn id="4" xr3:uid="{9C4F5506-B185-4F5A-92DE-87F5178FE86D}" name=" Team2             "/>
+    <tableColumn id="5" xr3:uid="{F6E15AFF-6DF0-46FA-873E-146D4E031966}" name="1"/>
+    <tableColumn id="6" xr3:uid="{37D4F760-2D02-4EF2-9B8F-2233A45C2633}" name="  N  "/>
+    <tableColumn id="7" xr3:uid="{71E729B9-1863-43DE-91C4-B5FFBA499023}" name="2"/>
+    <tableColumn id="8" xr3:uid="{746C6B52-B117-442F-945B-05E8133FAE08}" name="  p1   "/>
+    <tableColumn id="9" xr3:uid="{9C168FA0-300B-4747-AC65-D875C28578D8}" name="  pN   "/>
+    <tableColumn id="10" xr3:uid="{516C6D13-9328-4905-BA3F-5A5CEF01455D}" name="  p2   "/>
+    <tableColumn id="11" xr3:uid="{43C97C71-CE12-45A7-AD8C-91C1ED012CC7}" name="  c1   "/>
+    <tableColumn id="12" xr3:uid="{BDCD4592-1EDC-4A1F-92FF-B37D990291A9}" name="  cN   "/>
+    <tableColumn id="13" xr3:uid="{51BFB142-AEB2-4A01-A627-A0B874703E58}" name="  C2   "/>
+    <tableColumn id="14" xr3:uid="{41C34DE9-4BB6-472B-9D4D-44152836024D}" name="  1G   "/>
+    <tableColumn id="15" xr3:uid="{F0F52461-FFF4-4ED5-B698-021B55D73649}" name="  2G   "/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3C8709AF-EB7C-41AC-8155-F6ED1170DE24}" name="Tableau1" displayName="Tableau1" ref="A4:S36" totalsRowShown="0">
   <autoFilter ref="A4:S36" xr:uid="{F2F2D16C-230C-4CAC-A6FA-FA0A0D105F45}"/>
@@ -4877,7 +4960,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{338965B1-70E8-4C6E-9B36-81CFD9B4B68C}" name="Tableau2" displayName="Tableau2" ref="A38:M86" totalsRowShown="0">
   <autoFilter ref="A38:M86" xr:uid="{96ED0AB2-A97A-4D42-920C-6630AA3F4A02}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{A0A5A8FD-7607-48B6-9135-5D249D0BCE0F}" name="Date       " dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{A0A5A8FD-7607-48B6-9135-5D249D0BCE0F}" name="Date       " dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{E51B31D0-A0A3-4931-B875-C0BC5FD9B82D}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{C80B30D5-1BC2-4F07-B77C-972433CC014E}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{DA26DA73-82A9-49AC-BEE0-07CB81D8E66E}" name=" Team2             "/>
@@ -4930,7 +5013,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9A086498-695C-4792-B6A7-E6FA4AFD559A}" name="Tableau3" displayName="Tableau3" ref="A35:O83" totalsRowShown="0">
   <autoFilter ref="A35:O83" xr:uid="{A597B673-D5D6-41BB-8418-616CAD672A6C}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{28A461B9-B55B-45C3-A1C5-A72B63C0DE95}" name="Date       " dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{28A461B9-B55B-45C3-A1C5-A72B63C0DE95}" name="Date       " dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{4337CFE4-4E9E-483E-AB8D-9DE67C36B0A1}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{2182342D-CBD2-49C5-A25F-0F9C3CCD7107}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{85A22FCF-209F-43C5-A3D9-ABD31B6B3953}" name=" Team2             "/>
@@ -4986,7 +5069,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{6945C8BF-54A5-4025-8EA4-289C7FB8B708}" name="Tableau6" displayName="Tableau6" ref="A71:P119" totalsRowShown="0">
   <autoFilter ref="A71:P119" xr:uid="{9830D998-6315-4F2D-A674-5B740BF3E00C}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{6632B7A1-23F7-4D06-A323-51A64A023F48}" name="Date       " dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{6632B7A1-23F7-4D06-A323-51A64A023F48}" name="Date       " dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{20A74076-22FE-423D-8C0C-581C372EB016}" name="    Code    "/>
     <tableColumn id="3" xr3:uid="{A20C27C7-B5D8-4DF8-BD6B-E977DF554B7D}" name=" Team1             "/>
     <tableColumn id="4" xr3:uid="{F6FA5282-0C3B-4F38-93DE-4B7D0CC8DA41}" name=" Team2             "/>
@@ -10838,8 +10921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B031F157-2DBE-47F4-B3F1-B2831B36E5C8}">
   <dimension ref="A1:S68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13538,6 +13621,1455 @@
       </c>
       <c r="E68" t="s">
         <v>1430</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A510CA3-0147-4925-BEEB-4A526ABE1A31}">
+  <dimension ref="A1:S28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P31" sqref="P31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="3" max="4" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>2448</v>
+      </c>
+      <c r="C2">
+        <v>1090</v>
+      </c>
+      <c r="D2">
+        <v>3778</v>
+      </c>
+      <c r="E2">
+        <v>5386</v>
+      </c>
+      <c r="F2">
+        <v>8181</v>
+      </c>
+      <c r="G2">
+        <v>10000</v>
+      </c>
+      <c r="H2">
+        <v>24.5</v>
+      </c>
+      <c r="I2">
+        <v>10.9</v>
+      </c>
+      <c r="J2">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="K2">
+        <v>53.9</v>
+      </c>
+      <c r="L2">
+        <v>81.8</v>
+      </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+      <c r="N2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O2">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="P2">
+        <v>2.6</v>
+      </c>
+      <c r="Q2">
+        <v>1.9</v>
+      </c>
+      <c r="R2">
+        <v>1.2</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3">
+        <v>1444</v>
+      </c>
+      <c r="C3">
+        <v>1094</v>
+      </c>
+      <c r="D3">
+        <v>2959</v>
+      </c>
+      <c r="E3">
+        <v>4994</v>
+      </c>
+      <c r="F3">
+        <v>8346</v>
+      </c>
+      <c r="G3">
+        <v>10000</v>
+      </c>
+      <c r="H3">
+        <v>14.4</v>
+      </c>
+      <c r="I3">
+        <v>10.9</v>
+      </c>
+      <c r="J3">
+        <v>29.6</v>
+      </c>
+      <c r="K3">
+        <v>49.9</v>
+      </c>
+      <c r="L3">
+        <v>83.5</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>6.9</v>
+      </c>
+      <c r="O3">
+        <v>9.1</v>
+      </c>
+      <c r="P3">
+        <v>3.4</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>1.2</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1207</v>
+      </c>
+      <c r="C4">
+        <v>873</v>
+      </c>
+      <c r="D4">
+        <v>2232</v>
+      </c>
+      <c r="E4">
+        <v>3766</v>
+      </c>
+      <c r="F4">
+        <v>8763</v>
+      </c>
+      <c r="G4">
+        <v>10000</v>
+      </c>
+      <c r="H4">
+        <v>12.1</v>
+      </c>
+      <c r="I4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="J4">
+        <v>22.3</v>
+      </c>
+      <c r="K4">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="L4">
+        <v>87.6</v>
+      </c>
+      <c r="M4">
+        <v>100</v>
+      </c>
+      <c r="N4">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="O4">
+        <v>11.5</v>
+      </c>
+      <c r="P4">
+        <v>4.5</v>
+      </c>
+      <c r="Q4">
+        <v>2.7</v>
+      </c>
+      <c r="R4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>799</v>
+      </c>
+      <c r="C5">
+        <v>671</v>
+      </c>
+      <c r="D5">
+        <v>1684</v>
+      </c>
+      <c r="E5">
+        <v>3054</v>
+      </c>
+      <c r="F5">
+        <v>6226</v>
+      </c>
+      <c r="G5">
+        <v>10000</v>
+      </c>
+      <c r="H5">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>6.7</v>
+      </c>
+      <c r="J5">
+        <v>16.8</v>
+      </c>
+      <c r="K5">
+        <v>30.5</v>
+      </c>
+      <c r="L5">
+        <v>62.3</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <v>12.5</v>
+      </c>
+      <c r="O5">
+        <v>14.9</v>
+      </c>
+      <c r="P5">
+        <v>5.9</v>
+      </c>
+      <c r="Q5">
+        <v>3.3</v>
+      </c>
+      <c r="R5">
+        <v>1.6</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>781</v>
+      </c>
+      <c r="C6">
+        <v>861</v>
+      </c>
+      <c r="D6">
+        <v>1694</v>
+      </c>
+      <c r="E6">
+        <v>3427</v>
+      </c>
+      <c r="F6">
+        <v>6359</v>
+      </c>
+      <c r="G6">
+        <v>10000</v>
+      </c>
+      <c r="H6">
+        <v>7.8</v>
+      </c>
+      <c r="I6">
+        <v>8.6</v>
+      </c>
+      <c r="J6">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="K6">
+        <v>34.299999999999997</v>
+      </c>
+      <c r="L6">
+        <v>63.6</v>
+      </c>
+      <c r="M6">
+        <v>100</v>
+      </c>
+      <c r="N6">
+        <v>12.8</v>
+      </c>
+      <c r="O6">
+        <v>11.6</v>
+      </c>
+      <c r="P6">
+        <v>5.9</v>
+      </c>
+      <c r="Q6">
+        <v>2.9</v>
+      </c>
+      <c r="R6">
+        <v>1.6</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>670</v>
+      </c>
+      <c r="C7">
+        <v>1056</v>
+      </c>
+      <c r="D7">
+        <v>1321</v>
+      </c>
+      <c r="E7">
+        <v>3305</v>
+      </c>
+      <c r="F7">
+        <v>5461</v>
+      </c>
+      <c r="G7">
+        <v>10000</v>
+      </c>
+      <c r="H7">
+        <v>6.7</v>
+      </c>
+      <c r="I7">
+        <v>10.6</v>
+      </c>
+      <c r="J7">
+        <v>13.2</v>
+      </c>
+      <c r="K7">
+        <v>33.1</v>
+      </c>
+      <c r="L7">
+        <v>54.6</v>
+      </c>
+      <c r="M7">
+        <v>100</v>
+      </c>
+      <c r="N7">
+        <v>14.9</v>
+      </c>
+      <c r="O7">
+        <v>9.5</v>
+      </c>
+      <c r="P7">
+        <v>7.6</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>1.8</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>497</v>
+      </c>
+      <c r="C8">
+        <v>694</v>
+      </c>
+      <c r="D8">
+        <v>1197</v>
+      </c>
+      <c r="E8">
+        <v>2660</v>
+      </c>
+      <c r="F8">
+        <v>5214</v>
+      </c>
+      <c r="G8">
+        <v>10000</v>
+      </c>
+      <c r="H8">
+        <v>5</v>
+      </c>
+      <c r="I8">
+        <v>6.9</v>
+      </c>
+      <c r="J8">
+        <v>12</v>
+      </c>
+      <c r="K8">
+        <v>26.6</v>
+      </c>
+      <c r="L8">
+        <v>52.1</v>
+      </c>
+      <c r="M8">
+        <v>100</v>
+      </c>
+      <c r="N8">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="O8">
+        <v>14.4</v>
+      </c>
+      <c r="P8">
+        <v>8.4</v>
+      </c>
+      <c r="Q8">
+        <v>3.8</v>
+      </c>
+      <c r="R8">
+        <v>1.9</v>
+      </c>
+      <c r="S8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>488</v>
+      </c>
+      <c r="C9">
+        <v>591</v>
+      </c>
+      <c r="D9">
+        <v>1127</v>
+      </c>
+      <c r="E9">
+        <v>2439</v>
+      </c>
+      <c r="F9">
+        <v>4786</v>
+      </c>
+      <c r="G9">
+        <v>10000</v>
+      </c>
+      <c r="H9">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="I9">
+        <v>5.9</v>
+      </c>
+      <c r="J9">
+        <v>11.3</v>
+      </c>
+      <c r="K9">
+        <v>24.4</v>
+      </c>
+      <c r="L9">
+        <v>47.9</v>
+      </c>
+      <c r="M9">
+        <v>100</v>
+      </c>
+      <c r="N9">
+        <v>20.5</v>
+      </c>
+      <c r="O9">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="P9">
+        <v>8.9</v>
+      </c>
+      <c r="Q9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="R9">
+        <v>2.1</v>
+      </c>
+      <c r="S9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>453</v>
+      </c>
+      <c r="C10">
+        <v>828</v>
+      </c>
+      <c r="D10">
+        <v>937</v>
+      </c>
+      <c r="E10">
+        <v>2564</v>
+      </c>
+      <c r="F10">
+        <v>4539</v>
+      </c>
+      <c r="G10">
+        <v>10000</v>
+      </c>
+      <c r="H10">
+        <v>4.5</v>
+      </c>
+      <c r="I10">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="J10">
+        <v>9.4</v>
+      </c>
+      <c r="K10">
+        <v>25.6</v>
+      </c>
+      <c r="L10">
+        <v>45.4</v>
+      </c>
+      <c r="M10">
+        <v>100</v>
+      </c>
+      <c r="N10">
+        <v>22.1</v>
+      </c>
+      <c r="O10">
+        <v>12.1</v>
+      </c>
+      <c r="P10">
+        <v>10.7</v>
+      </c>
+      <c r="Q10">
+        <v>3.9</v>
+      </c>
+      <c r="R10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>404</v>
+      </c>
+      <c r="C11">
+        <v>775</v>
+      </c>
+      <c r="D11">
+        <v>896</v>
+      </c>
+      <c r="E11">
+        <v>2500</v>
+      </c>
+      <c r="F11">
+        <v>5622</v>
+      </c>
+      <c r="G11">
+        <v>10000</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>7.8</v>
+      </c>
+      <c r="J11">
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <v>25</v>
+      </c>
+      <c r="L11">
+        <v>56.2</v>
+      </c>
+      <c r="M11">
+        <v>100</v>
+      </c>
+      <c r="N11">
+        <v>24.8</v>
+      </c>
+      <c r="O11">
+        <v>12.9</v>
+      </c>
+      <c r="P11">
+        <v>11.2</v>
+      </c>
+      <c r="Q11">
+        <v>4</v>
+      </c>
+      <c r="R11">
+        <v>1.8</v>
+      </c>
+      <c r="S11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>224</v>
+      </c>
+      <c r="C12">
+        <v>336</v>
+      </c>
+      <c r="D12">
+        <v>585</v>
+      </c>
+      <c r="E12">
+        <v>1474</v>
+      </c>
+      <c r="F12">
+        <v>3641</v>
+      </c>
+      <c r="G12">
+        <v>10000</v>
+      </c>
+      <c r="H12">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I12">
+        <v>3.4</v>
+      </c>
+      <c r="J12">
+        <v>5.9</v>
+      </c>
+      <c r="K12">
+        <v>14.7</v>
+      </c>
+      <c r="L12">
+        <v>36.4</v>
+      </c>
+      <c r="M12">
+        <v>100</v>
+      </c>
+      <c r="N12">
+        <v>44.6</v>
+      </c>
+      <c r="O12">
+        <v>29.8</v>
+      </c>
+      <c r="P12">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="Q12">
+        <v>6.8</v>
+      </c>
+      <c r="R12">
+        <v>2.7</v>
+      </c>
+      <c r="S12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>222</v>
+      </c>
+      <c r="C13">
+        <v>341</v>
+      </c>
+      <c r="D13">
+        <v>628</v>
+      </c>
+      <c r="E13">
+        <v>1472</v>
+      </c>
+      <c r="F13">
+        <v>3774</v>
+      </c>
+      <c r="G13">
+        <v>10000</v>
+      </c>
+      <c r="H13">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I13">
+        <v>3.4</v>
+      </c>
+      <c r="J13">
+        <v>6.3</v>
+      </c>
+      <c r="K13">
+        <v>14.7</v>
+      </c>
+      <c r="L13">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13">
+        <v>45</v>
+      </c>
+      <c r="O13">
+        <v>29.3</v>
+      </c>
+      <c r="P13">
+        <v>15.9</v>
+      </c>
+      <c r="Q13">
+        <v>6.8</v>
+      </c>
+      <c r="R13">
+        <v>2.6</v>
+      </c>
+      <c r="S13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14">
+        <v>194</v>
+      </c>
+      <c r="C14">
+        <v>513</v>
+      </c>
+      <c r="D14">
+        <v>488</v>
+      </c>
+      <c r="E14">
+        <v>1631</v>
+      </c>
+      <c r="F14">
+        <v>4378</v>
+      </c>
+      <c r="G14">
+        <v>10000</v>
+      </c>
+      <c r="H14">
+        <v>1.9</v>
+      </c>
+      <c r="I14">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="J14">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K14">
+        <v>16.3</v>
+      </c>
+      <c r="L14">
+        <v>43.8</v>
+      </c>
+      <c r="M14">
+        <v>100</v>
+      </c>
+      <c r="N14">
+        <v>51.5</v>
+      </c>
+      <c r="O14">
+        <v>19.5</v>
+      </c>
+      <c r="P14">
+        <v>20.5</v>
+      </c>
+      <c r="Q14">
+        <v>6.1</v>
+      </c>
+      <c r="R14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>122</v>
+      </c>
+      <c r="C15">
+        <v>145</v>
+      </c>
+      <c r="D15">
+        <v>290</v>
+      </c>
+      <c r="E15">
+        <v>663</v>
+      </c>
+      <c r="F15">
+        <v>1819</v>
+      </c>
+      <c r="G15">
+        <v>10000</v>
+      </c>
+      <c r="H15">
+        <v>1.2</v>
+      </c>
+      <c r="I15">
+        <v>1.5</v>
+      </c>
+      <c r="J15">
+        <v>2.9</v>
+      </c>
+      <c r="K15">
+        <v>6.6</v>
+      </c>
+      <c r="L15">
+        <v>18.2</v>
+      </c>
+      <c r="M15">
+        <v>100</v>
+      </c>
+      <c r="N15">
+        <v>82</v>
+      </c>
+      <c r="O15">
+        <v>69</v>
+      </c>
+      <c r="P15">
+        <v>34.5</v>
+      </c>
+      <c r="Q15">
+        <v>15.1</v>
+      </c>
+      <c r="R15">
+        <v>5.5</v>
+      </c>
+      <c r="S15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16">
+        <v>101</v>
+      </c>
+      <c r="D16">
+        <v>126</v>
+      </c>
+      <c r="E16">
+        <v>480</v>
+      </c>
+      <c r="F16">
+        <v>1654</v>
+      </c>
+      <c r="G16">
+        <v>10000</v>
+      </c>
+      <c r="H16">
+        <v>0.3</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1.3</v>
+      </c>
+      <c r="K16">
+        <v>4.8</v>
+      </c>
+      <c r="L16">
+        <v>16.5</v>
+      </c>
+      <c r="M16">
+        <v>100</v>
+      </c>
+      <c r="N16">
+        <v>333.3</v>
+      </c>
+      <c r="O16">
+        <v>99</v>
+      </c>
+      <c r="P16">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="Q16">
+        <v>20.8</v>
+      </c>
+      <c r="R16">
+        <v>6</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>31</v>
+      </c>
+      <c r="D17">
+        <v>58</v>
+      </c>
+      <c r="E17">
+        <v>185</v>
+      </c>
+      <c r="F17">
+        <v>1237</v>
+      </c>
+      <c r="G17">
+        <v>10000</v>
+      </c>
+      <c r="H17">
+        <v>0.2</v>
+      </c>
+      <c r="I17">
+        <v>0.3</v>
+      </c>
+      <c r="J17">
+        <v>0.6</v>
+      </c>
+      <c r="K17">
+        <v>1.8</v>
+      </c>
+      <c r="L17">
+        <v>12.4</v>
+      </c>
+      <c r="M17">
+        <v>100</v>
+      </c>
+      <c r="N17">
+        <v>588.20000000000005</v>
+      </c>
+      <c r="O17">
+        <v>322.60000000000002</v>
+      </c>
+      <c r="P17">
+        <v>172.4</v>
+      </c>
+      <c r="Q17">
+        <v>54.1</v>
+      </c>
+      <c r="R17">
+        <v>8.1</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" t="s">
+        <v>55</v>
+      </c>
+      <c r="G20" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" t="s">
+        <v>56</v>
+      </c>
+      <c r="J20" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" t="s">
+        <v>57</v>
+      </c>
+      <c r="M20" t="s">
+        <v>58</v>
+      </c>
+      <c r="N20" t="s">
+        <v>255</v>
+      </c>
+      <c r="O20" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43281</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1431</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21">
+        <v>4786</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>5214</v>
+      </c>
+      <c r="H21">
+        <v>47.9</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>52.1</v>
+      </c>
+      <c r="K21">
+        <v>2.1</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1.9</v>
+      </c>
+      <c r="N21">
+        <v>1.8</v>
+      </c>
+      <c r="O21">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43281</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1432</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22">
+        <v>6359</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>3641</v>
+      </c>
+      <c r="H22">
+        <v>63.6</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>36.4</v>
+      </c>
+      <c r="K22">
+        <v>1.6</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>2.7</v>
+      </c>
+      <c r="N22">
+        <v>2</v>
+      </c>
+      <c r="O22">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1433</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23">
+        <v>8346</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>1654</v>
+      </c>
+      <c r="H23">
+        <v>83.5</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>16.5</v>
+      </c>
+      <c r="K23">
+        <v>1.2</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>6</v>
+      </c>
+      <c r="N23">
+        <v>2.5</v>
+      </c>
+      <c r="O23">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43282</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1434</v>
+      </c>
+      <c r="C24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24">
+        <v>6226</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>3774</v>
+      </c>
+      <c r="H24">
+        <v>62.3</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="K24">
+        <v>1.6</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>2.6</v>
+      </c>
+      <c r="N24">
+        <v>2</v>
+      </c>
+      <c r="O24">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43283</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25">
+        <v>8181</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>1819</v>
+      </c>
+      <c r="H25">
+        <v>81.8</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>18.2</v>
+      </c>
+      <c r="K25">
+        <v>1.2</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>5.5</v>
+      </c>
+      <c r="N25">
+        <v>2.4</v>
+      </c>
+      <c r="O25">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43283</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1436</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26">
+        <v>8763</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>1237</v>
+      </c>
+      <c r="H26">
+        <v>87.6</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>12.4</v>
+      </c>
+      <c r="K26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>8.1</v>
+      </c>
+      <c r="N26">
+        <v>2.5</v>
+      </c>
+      <c r="O26">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43284</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1437</v>
+      </c>
+      <c r="C27" t="s">
+        <v>96</v>
+      </c>
+      <c r="D27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27">
+        <v>4378</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>5622</v>
+      </c>
+      <c r="H27">
+        <v>43.8</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>56.2</v>
+      </c>
+      <c r="K27">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>1.8</v>
+      </c>
+      <c r="N27">
+        <v>1.7</v>
+      </c>
+      <c r="O27">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43284</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1438</v>
+      </c>
+      <c r="C28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28">
+        <v>4539</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>5461</v>
+      </c>
+      <c r="H28">
+        <v>45.4</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>54.6</v>
+      </c>
+      <c r="K28">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>1.8</v>
+      </c>
+      <c r="N28">
+        <v>1.7</v>
+      </c>
+      <c r="O28">
+        <v>1.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>